<commit_message>
Finished with everyone's presentations and edits
</commit_message>
<xml_diff>
--- a/tables/Majors.xlsx
+++ b/tables/Majors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volun\Documents\DA9\Capstone\capstone_da9_chase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\volun\Documents\DA9\Capstone\capstone_da9_chase\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CB94526-3442-4183-B5A4-791F69FFAB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C28E32-FBFA-4809-84B7-3B9B93BFBB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Majors" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <t>Major</t>
   </si>
   <si>
-    <t>All Majors Combined</t>
-  </si>
-  <si>
     <t>Bachelor's in Biological Agricultural and Environmental Sciences</t>
   </si>
   <si>
@@ -71,12 +68,15 @@
   </si>
   <si>
     <t>Bachelor's in Visual and Performing Arts</t>
+  </si>
+  <si>
+    <t>Bachelor's in All Majors Combined</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -910,10 +910,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -924,82 +926,82 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>